<commit_message>
Changed the fixed voltage regulator to AMS1117/LM1117 and the output capacitor.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="96">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">E2,5-6</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C2</t>
+    <t xml:space="preserve">C1</t>
   </si>
   <si>
     <t xml:space="preserve">POLARIZED CAPACITOR, European symbol</t>
@@ -157,6 +157,15 @@
     <t xml:space="preserve">RAD FR 100/16</t>
   </si>
   <si>
+    <t xml:space="preserve">22µF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T350 22U 16</t>
+  </si>
+  <si>
     <t xml:space="preserve">10k</t>
   </si>
   <si>
@@ -241,10 +250,10 @@
     <t xml:space="preserve">JST XH5P ST </t>
   </si>
   <si>
-    <t xml:space="preserve">LM3940</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UA78M33DCY</t>
+    <t xml:space="preserve">AMS1117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LM1117IMPX-3.3</t>
   </si>
   <si>
     <t xml:space="preserve">SOT223</t>
@@ -256,7 +265,7 @@
     <t xml:space="preserve">POSITIVE-VOLTAGE REGULATORS</t>
   </si>
   <si>
-    <t xml:space="preserve">LM 3940 IMP-3,3</t>
+    <t xml:space="preserve">LM 1117 MPX-3.3</t>
   </si>
   <si>
     <t xml:space="preserve">MA05-1_WON</t>
@@ -308,11 +317,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -328,6 +338,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -372,8 +387,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -398,17 +417,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="69.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.84"/>
@@ -616,7 +635,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>39</v>
@@ -645,18 +664,18 @@
         <v>45</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>47</v>
       </c>
     </row>
@@ -668,19 +687,19 @@
         <v>48</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="F13" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,53 +707,53 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="E14" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="F14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B15" s="0" t="n">
-        <v>390</v>
+      <c r="B15" s="0" t="s">
+        <v>55</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>58</v>
+      <c r="G15" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>59</v>
+      <c r="B16" s="0" t="n">
+        <v>390</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>26</v>
@@ -748,7 +767,7 @@
       <c r="F16" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -760,30 +779,36 @@
         <v>62</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>63</v>
       </c>
+      <c r="F17" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,16 +816,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -808,10 +833,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>69</v>
@@ -819,50 +844,47 @@
       <c r="E20" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="F21" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="G21" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" s="0" t="s">
+      <c r="F22" s="0" t="s">
         <v>80</v>
       </c>
       <c r="G22" s="0" t="s">
@@ -871,7 +893,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>82</v>
@@ -880,16 +902,13 @@
         <v>82</v>
       </c>
       <c r="D23" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="G23" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H23" s="0" t="n">
-        <v>1605564</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -897,10 +916,10 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>86</v>
@@ -908,24 +927,27 @@
       <c r="E24" s="0" t="s">
         <v>87</v>
       </c>
+      <c r="F24" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>1605564</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="F25" s="0" t="s">
         <v>90</v>
       </c>
     </row>
@@ -933,11 +955,31 @@
       <c r="A26" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B26" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>92</v>
+      </c>
       <c r="F26" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>